<commit_message>
📦 Update in code for github
</commit_message>
<xml_diff>
--- a/Criativa.xlsx
+++ b/Criativa.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E35"/>
+  <dimension ref="A1:F35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,12 +437,13 @@
           <t>Geração Diaria</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
+      <c r="D1" t="inlineStr"/>
+      <c r="E1" t="inlineStr">
         <is>
           <t>Clima</t>
         </is>
       </c>
-      <c r="E1" t="inlineStr">
+      <c r="F1" t="inlineStr">
         <is>
           <t>Data/Hora</t>
         </is>
@@ -451,25 +452,30 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>GSM Márcio Curty</t>
+          <t>SFV_Compromisso Ambiental</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Estrada Nova Aurora, 4038, Carmo - RJ, CEP 28.640-000</t>
+          <t>Av. Augusto Perácio, 246 – CEP 36660-000, São Luiz, Além Paraíba – MG</t>
         </is>
       </c>
       <c r="C2">
-        <f>VALOR(0</f>
-        <v/>
-      </c>
-      <c r="D2">
-        <f>IMAGEM("https://static.semsportal.com/static/Images/icon-weather-new/101.png";"CLIMA")</f>
-        <v/>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>10/11/2023, 02:01</t>
+        <f>VALOR(370.1)</f>
+        <v/>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>https://static.semsportal.com/static/Images/icon-weather-new/101.png</t>
+        </is>
+      </c>
+      <c r="E2">
+        <f>IMAGEM(D2;"CLIMA")</f>
+        <v/>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>10/11/2023, 18:58</t>
         </is>
       </c>
     </row>
@@ -485,216 +491,261 @@
         </is>
       </c>
       <c r="C3">
-        <f>VALOR(1678</f>
-        <v/>
-      </c>
-      <c r="D3">
-        <f>IMAGEM("https://static.semsportal.com/static/Images/icon-weather-new/101.png";"CLIMA")</f>
-        <v/>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>10/11/2023, 02:01</t>
+        <f>VALOR(1564.7)</f>
+        <v/>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>https://static.semsportal.com/static/Images/icon-weather-new/101.png</t>
+        </is>
+      </c>
+      <c r="E3">
+        <f>IMAGEM(D3;"CLIMA")</f>
+        <v/>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>10/11/2023, 18:58</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>SFV_Compromisso Ambiental</t>
+          <t>SFV_Igor Navarro</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Av. Augusto Perácio, 246 – CEP 36660-000, São Luiz, Além Paraíba – MG</t>
+          <t>RUA PEDRO BRAZ DA SILVA, 7, NOVA NITEROI, TRÊS RIOS - RJ</t>
         </is>
       </c>
       <c r="C4">
-        <f>VALOR(474</f>
-        <v/>
-      </c>
-      <c r="D4">
-        <f>IMAGEM("https://static.semsportal.com/static/Images/icon-weather-new/101.png";"CLIMA")</f>
-        <v/>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>10/11/2023, 02:01</t>
+        <f>VALOR(80.2)</f>
+        <v/>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>https://static.semsportal.com/static/Images/icon-weather-new/101.png</t>
+        </is>
+      </c>
+      <c r="E4">
+        <f>IMAGEM(D4;"CLIMA")</f>
+        <v/>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>10/11/2023, 18:58</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>SFV_Igor Navarro</t>
+          <t>UFV Santa Cecília III</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>RUA PEDRO BRAZ DA SILVA, 7, NOVA NITEROI, TRÊS RIOS - RJ</t>
+          <t>Estrada Fazenda Santa Terezinha, 578D, Boa Esperança, Mendes – RJ, CEP:  26.700-000</t>
         </is>
       </c>
       <c r="C5">
-        <f>VALOR(86</f>
-        <v/>
-      </c>
-      <c r="D5">
-        <f>IMAGEM("https://static.semsportal.com/static/Images/icon-weather-new/101.png";"CLIMA")</f>
-        <v/>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>10/11/2023, 02:01</t>
+        <f>VALOR(520.4)</f>
+        <v/>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>https://static.semsportal.com/static/Images/icon-weather-new/101.png</t>
+        </is>
+      </c>
+      <c r="E5">
+        <f>IMAGEM(D5;"CLIMA")</f>
+        <v/>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>10/11/2023, 18:58</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>SFV_Gemapel</t>
+          <t>GSM MÁRCIA CURTY</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>AVENIDA FRANCISCO VALADARES, 24 GALPÃO 109, POÇO RICO, JUIZ DE FORA - MG</t>
+          <t>Estrada Nova Aurora, 4020, bairro Aurora, Carmo-RJ, CEP 28.640-000</t>
         </is>
       </c>
       <c r="C6">
-        <f>VALOR(51</f>
-        <v/>
-      </c>
-      <c r="D6">
-        <f>IMAGEM("https://static.semsportal.com/static/Images/icon-weather-new/101.png";"CLIMA")</f>
-        <v/>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>10/11/2023, 02:01</t>
+        <f>VALOR(532.5)</f>
+        <v/>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>https://static.semsportal.com/static/Images/icon-weather-new/101.png</t>
+        </is>
+      </c>
+      <c r="E6">
+        <f>IMAGEM(D6;"CLIMA")</f>
+        <v/>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>10/11/2023, 18:58</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>UFV Santa Luiza I</t>
+          <t>São Francisco I</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Fazenda santa Luiza , Rio das Flores, rio de janeiro</t>
+          <t>Rio Claro</t>
         </is>
       </c>
       <c r="C7">
-        <f>VALOR(568</f>
-        <v/>
-      </c>
-      <c r="D7">
-        <f>IMAGEM("https://static.semsportal.com/static/Images/icon-weather-new/101.png";"CLIMA")</f>
-        <v/>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>10/11/2023, 02:01</t>
+        <f>VALOR(554.2)</f>
+        <v/>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>https://static.semsportal.com/static/Images/icon-weather-new/101.png</t>
+        </is>
+      </c>
+      <c r="E7">
+        <f>IMAGEM(D7;"CLIMA")</f>
+        <v/>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>10/11/2023, 18:58</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>GSM MÁRCIA CURTY</t>
+          <t>SFV_Gemapel</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Estrada Nova Aurora, 4020, bairro Aurora, Carmo-RJ, CEP 28.640-000</t>
+          <t>AVENIDA FRANCISCO VALADARES, 24 GALPÃO 109, POÇO RICO, JUIZ DE FORA - MG</t>
         </is>
       </c>
       <c r="C8">
-        <f>VALOR(564</f>
-        <v/>
-      </c>
-      <c r="D8">
-        <f>IMAGEM("https://static.semsportal.com/static/Images/icon-weather-new/101.png";"CLIMA")</f>
-        <v/>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>10/11/2023, 02:01</t>
+        <f>VALOR(51.0)</f>
+        <v/>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>https://static.semsportal.com/static/Images/icon-weather-new/101.png</t>
+        </is>
+      </c>
+      <c r="E8">
+        <f>IMAGEM(D8;"CLIMA")</f>
+        <v/>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>10/11/2023, 18:58</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>GSM SÍTIO CAMPO ALEGRE II</t>
+          <t>UFV Santa Luiza I</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Estrada Sumidouro, 1660, CA, Bairro Jamapará, Sapucaia/</t>
+          <t>Fazenda santa Luiza , Rio das Flores, rio de janeiro</t>
         </is>
       </c>
       <c r="C9">
-        <f>VALOR(589</f>
-        <v/>
-      </c>
-      <c r="D9">
-        <f>IMAGEM("https://static.semsportal.com/static/Images/icon-weather-new/101.png";"CLIMA")</f>
-        <v/>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>10/11/2023, 02:01</t>
+        <f>VALOR(565.6)</f>
+        <v/>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>https://static.semsportal.com/static/Images/icon-weather-new/101.png</t>
+        </is>
+      </c>
+      <c r="E9">
+        <f>IMAGEM(D9;"CLIMA")</f>
+        <v/>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>10/11/2023, 18:58</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>São Francisco I</t>
+          <t>GSM SÍTIO CAMPO ALEGRE II</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Rio Claro</t>
+          <t>Estrada Sumidouro, 1660, CA, Bairro Jamapará, Sapucaia/</t>
         </is>
       </c>
       <c r="C10">
-        <f>VALOR(598</f>
-        <v/>
-      </c>
-      <c r="D10">
-        <f>IMAGEM("https://static.semsportal.com/static/Images/icon-weather-new/101.png";"CLIMA")</f>
-        <v/>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>10/11/2023, 02:01</t>
+        <f>VALOR(569.0)</f>
+        <v/>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>https://static.semsportal.com/static/Images/icon-weather-new/101.png</t>
+        </is>
+      </c>
+      <c r="E10">
+        <f>IMAGEM(D10;"CLIMA")</f>
+        <v/>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>10/11/2023, 18:58</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>UFV Santa Cecília III</t>
+          <t>GSM Cel Abílio 25kW</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Estrada Fazenda Santa Terezinha, 578D, Boa Esperança, Mendes – RJ, CEP:  26.700-000</t>
+          <t>R. Cel. Abílio Herdy Alves, 150</t>
         </is>
       </c>
       <c r="C11">
-        <f>VALOR(604</f>
-        <v/>
-      </c>
-      <c r="D11">
-        <f>IMAGEM("https://static.semsportal.com/static/Images/icon-weather-new/101.png";"CLIMA")</f>
-        <v/>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>10/11/2023, 02:01</t>
+        <f>VALOR(72.8)</f>
+        <v/>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>https://static.semsportal.com/static/Images/icon-weather-new/101.png</t>
+        </is>
+      </c>
+      <c r="E11">
+        <f>IMAGEM(D11;"CLIMA")</f>
+        <v/>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>10/11/2023, 18:58</t>
         </is>
       </c>
     </row>
@@ -710,98 +761,118 @@
         </is>
       </c>
       <c r="C12">
-        <f>VALOR(617</f>
-        <v/>
-      </c>
-      <c r="D12">
-        <f>IMAGEM("https://static.semsportal.com/static/Images/icon-weather-new/101.png";"CLIMA")</f>
-        <v/>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>10/11/2023, 02:01</t>
+        <f>VALOR(599.2)</f>
+        <v/>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>https://static.semsportal.com/static/Images/icon-weather-new/101.png</t>
+        </is>
+      </c>
+      <c r="E12">
+        <f>IMAGEM(D12;"CLIMA")</f>
+        <v/>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>10/11/2023, 18:58</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>GSM Cel Abílio 25kW</t>
+          <t>GSM Lote 12</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>R. Cel. Abílio Herdy Alves, 150</t>
+          <t>Avenida Avelino Salatiel, 12, Santana do Deserto - MG</t>
         </is>
       </c>
       <c r="C13">
-        <f>VALOR(77</f>
-        <v/>
-      </c>
-      <c r="D13">
-        <f>IMAGEM("https://static.semsportal.com/static/Images/icon-weather-new/101.png";"CLIMA")</f>
-        <v/>
-      </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>10/11/2023, 02:01</t>
+        <f>VALOR(601.8)</f>
+        <v/>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>https://static.semsportal.com/static/Images/icon-weather-new/101.png</t>
+        </is>
+      </c>
+      <c r="E13">
+        <f>IMAGEM(D13;"CLIMA")</f>
+        <v/>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>10/11/2023, 18:58</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>GSM Lote 12</t>
+          <t>FOT Lote 27</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Avenida Avelino Salatiel, 12, Santana do Deserto - MG</t>
+          <t>Rua A, nº27, Quadra B, Loteamento Portal de Belmiro Braga II, Belmiro Braga – MG, CEP: 36.126-000</t>
         </is>
       </c>
       <c r="C14">
-        <f>VALOR(624</f>
-        <v/>
-      </c>
-      <c r="D14">
-        <f>IMAGEM("https://static.semsportal.com/static/Images/icon-weather-new/101.png";"CLIMA")</f>
-        <v/>
-      </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>10/11/2023, 02:01</t>
+        <f>VALOR(482.6)</f>
+        <v/>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>https://static.semsportal.com/static/Images/icon-weather-new/101.png</t>
+        </is>
+      </c>
+      <c r="E14">
+        <f>IMAGEM(D14;"CLIMA")</f>
+        <v/>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>10/11/2023, 18:58</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>FOT Lote 27</t>
+          <t>GSM Marcus Curty</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Rua A, nº27, Quadra B, Loteamento Portal de Belmiro Braga II, Belmiro Braga – MG, CEP: 36.126-000</t>
+          <t>Estrada Nova Aurora, 4038, Carmo - RJ, CEP 28.640-000</t>
         </is>
       </c>
       <c r="C15">
-        <f>VALOR(513</f>
-        <v/>
-      </c>
-      <c r="D15">
-        <f>IMAGEM("https://static.semsportal.com/static/Images/icon-weather-new/101.png";"CLIMA")</f>
-        <v/>
-      </c>
-      <c r="E15" t="inlineStr">
-        <is>
-          <t>10/11/2023, 02:01</t>
+        <f>VALOR(498.7)</f>
+        <v/>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>https://static.semsportal.com/static/Images/icon-weather-new/101.png</t>
+        </is>
+      </c>
+      <c r="E15">
+        <f>IMAGEM(D15;"CLIMA")</f>
+        <v/>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>10/11/2023, 18:58</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>GSM Marcus Curty</t>
+          <t>GSM Márcio Curty</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -810,16 +881,21 @@
         </is>
       </c>
       <c r="C16">
-        <f>VALOR(526</f>
-        <v/>
-      </c>
-      <c r="D16">
-        <f>IMAGEM("https://static.semsportal.com/static/Images/icon-weather-new/101.png";"CLIMA")</f>
-        <v/>
-      </c>
-      <c r="E16" t="inlineStr">
-        <is>
-          <t>10/11/2023, 02:01</t>
+        <f>VALOR(626.8)</f>
+        <v/>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>https://static.semsportal.com/static/Images/icon-weather-new/101.png</t>
+        </is>
+      </c>
+      <c r="E16">
+        <f>IMAGEM(D16;"CLIMA")</f>
+        <v/>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>10/11/2023, 18:58</t>
         </is>
       </c>
     </row>
@@ -835,28 +911,33 @@
         </is>
       </c>
       <c r="C17">
-        <f>VALOR(601</f>
-        <v/>
-      </c>
-      <c r="D17">
-        <f>IMAGEM("https://static.semsportal.com/static/Images/icon-weather-new/101.png";"CLIMA")</f>
-        <v/>
-      </c>
-      <c r="E17" t="inlineStr">
-        <is>
-          <t>10/11/2023, 02:01</t>
+        <f>VALOR(581.7)</f>
+        <v/>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>https://static.semsportal.com/static/Images/icon-weather-new/101.png</t>
+        </is>
+      </c>
+      <c r="E17">
+        <f>IMAGEM(D17;"CLIMA")</f>
+        <v/>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>10/11/2023, 18:58</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Campo Belo I</t>
+          <t>Olaria CX 1</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Pequeri, State of Minas Gerais, 36610-000, Brazil</t>
+          <t>Sitio Olaria 9999 CX 1, Área Rural, Pequeri - MG</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -864,43 +945,43 @@
           <t>0,00</t>
         </is>
       </c>
-      <c r="E18" t="inlineStr">
-        <is>
-          <t>10/11/2023, 02:01</t>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>10/11/2023, 18:58</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Cel. Abilio</t>
+          <t>Santa Cecilia II</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Estr. Pequeri - Sarandira, Pequeri - MG, 36610-000, Brazil</t>
+          <t>Estrada Fazenda Santa Terezinha, 578 C, Boa Esperança, Mendes – RJ</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>0,00</t>
-        </is>
-      </c>
-      <c r="E19" t="inlineStr">
-        <is>
-          <t>10/11/2023, 02:01</t>
+          <t>47,30</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>10/11/2023, 18:58</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Lote 14</t>
+          <t>São Francisco II</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>AV. SALATIEL LOBATO (LOTE14) - SANTANA DO DESERTO</t>
+          <t>Estr. Moçambique, Areal - RJ, 25845-000, Brasil</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
@@ -908,119 +989,119 @@
           <t>0,00</t>
         </is>
       </c>
-      <c r="E20" t="inlineStr">
-        <is>
-          <t>10/11/2023, 02:01</t>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>10/11/2023, 18:58</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Olaria CX 1</t>
+          <t>Pequeri I</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Sitio Olaria 9999 CX 1, Área Rural, Pequeri - MG</t>
+          <t>Minas Gerais,Brazil</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>0,00</t>
-        </is>
-      </c>
-      <c r="E21" t="inlineStr">
-        <is>
-          <t>10/11/2023, 02:01</t>
+          <t>67,30</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>10/11/2023, 18:58</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Olaria CX2</t>
+          <t>Campo Belo I</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Sitio Olaria 9999 CX 2, Área Rural, Pequeri - MG</t>
+          <t>Pequeri, State of Minas Gerais, 36610-000, Brazil</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>0,00</t>
-        </is>
-      </c>
-      <c r="E22" t="inlineStr">
-        <is>
-          <t>10/11/2023, 02:01</t>
+          <t>349,20</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>10/11/2023, 18:58</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Pequeri I</t>
+          <t>Cel. Abilio</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Minas Gerais,Brazil</t>
+          <t>Estr. Pequeri - Sarandira, Pequeri - MG, 36610-000, Brazil</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>0,00</t>
-        </is>
-      </c>
-      <c r="E23" t="inlineStr">
-        <is>
-          <t>10/11/2023, 02:01</t>
+          <t>306,30</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>10/11/2023, 18:58</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Santa Cecilia II</t>
+          <t>Lote 14</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Estrada Fazenda Santa Terezinha, 578 C, Boa Esperança, Mendes – RJ</t>
+          <t>AV. SALATIEL LOBATO (LOTE14) - SANTANA DO DESERTO</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>0,00</t>
-        </is>
-      </c>
-      <c r="E24" t="inlineStr">
-        <is>
-          <t>10/11/2023, 02:01</t>
+          <t>451,90</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>10/11/2023, 18:58</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>São Francisco II</t>
+          <t>Olaria CX2</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Estr. Moçambique, Areal - RJ, 25845-000, Brasil</t>
+          <t>Sitio Olaria 9999 CX 2, Área Rural, Pequeri - MG</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>0,00</t>
-        </is>
-      </c>
-      <c r="E25" t="inlineStr">
-        <is>
-          <t>10/11/2023, 02:01</t>
+          <t>37,30</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>10/11/2023, 18:58</t>
         </is>
       </c>
     </row>
@@ -1037,12 +1118,12 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>0,00</t>
-        </is>
-      </c>
-      <c r="E26" t="inlineStr">
-        <is>
-          <t>10/11/2023, 02:01</t>
+          <t>480,86</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>10/11/2023, 18:58</t>
         </is>
       </c>
     </row>
@@ -1059,12 +1140,12 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t xml:space="preserve">0 </t>
-        </is>
-      </c>
-      <c r="E27" t="inlineStr">
-        <is>
-          <t>10/11/2023, 02:01</t>
+          <t xml:space="preserve">488,6 </t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>10/11/2023, 18:58</t>
         </is>
       </c>
     </row>
@@ -1081,12 +1162,12 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t xml:space="preserve">0 </t>
-        </is>
-      </c>
-      <c r="E28" t="inlineStr">
-        <is>
-          <t>10/11/2023, 02:01</t>
+          <t xml:space="preserve">160 </t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>10/11/2023, 18:58</t>
         </is>
       </c>
     </row>
@@ -1103,12 +1184,12 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t xml:space="preserve">0 </t>
-        </is>
-      </c>
-      <c r="E29" t="inlineStr">
-        <is>
-          <t>10/11/2023, 02:01</t>
+          <t xml:space="preserve">544,1 </t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>10/11/2023, 18:58</t>
         </is>
       </c>
     </row>
@@ -1125,12 +1206,12 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t xml:space="preserve">0 </t>
-        </is>
-      </c>
-      <c r="E30" t="inlineStr">
-        <is>
-          <t>10/11/2023, 02:01</t>
+          <t xml:space="preserve">58,7 </t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>10/11/2023, 18:58</t>
         </is>
       </c>
     </row>
@@ -1147,12 +1228,12 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t xml:space="preserve">0 </t>
-        </is>
-      </c>
-      <c r="E31" t="inlineStr">
-        <is>
-          <t>10/11/2023, 02:01</t>
+          <t xml:space="preserve">556,4 </t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>10/11/2023, 18:58</t>
         </is>
       </c>
     </row>
@@ -1169,12 +1250,12 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t xml:space="preserve">0 </t>
-        </is>
-      </c>
-      <c r="E32" t="inlineStr">
-        <is>
-          <t>10/11/2023, 02:01</t>
+          <t xml:space="preserve">110 </t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>10/11/2023, 18:58</t>
         </is>
       </c>
     </row>
@@ -1194,9 +1275,9 @@
           <t xml:space="preserve">0 </t>
         </is>
       </c>
-      <c r="E33" t="inlineStr">
-        <is>
-          <t>10/11/2023, 02:01</t>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>10/11/2023, 18:58</t>
         </is>
       </c>
     </row>
@@ -1216,9 +1297,9 @@
           <t xml:space="preserve">0 </t>
         </is>
       </c>
-      <c r="E34" t="inlineStr">
-        <is>
-          <t>10/11/2023, 02:01</t>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>10/11/2023, 18:58</t>
         </is>
       </c>
     </row>
@@ -1235,12 +1316,12 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t xml:space="preserve">0 </t>
-        </is>
-      </c>
-      <c r="E35" t="inlineStr">
-        <is>
-          <t>10/11/2023, 02:01</t>
+          <t xml:space="preserve">287,2 </t>
+        </is>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>10/11/2023, 18:58</t>
         </is>
       </c>
     </row>

</xml_diff>